<commit_message>
delete, update customer by id excel
</commit_message>
<xml_diff>
--- a/dulieu/khachHangOutput.xlsx
+++ b/dulieu/khachHangOutput.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>ID Khách Hàng</t>
   </si>
@@ -32,6 +32,18 @@
     <t>1</t>
   </si>
   <si>
+    <t>hung</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>123123123123</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>Huy</t>
   </si>
   <si>
@@ -41,19 +53,10 @@
     <t>042203013460</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
     <t>Hai</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>123123123123</t>
   </si>
   <si>
     <t>4</t>
@@ -113,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -157,7 +160,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -165,13 +168,13 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -179,10 +182,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -191,40 +194,23 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>